<commit_message>
Update women registration form
</commit_message>
<xml_diff>
--- a/setuper/data/registration_vaccination_pregnant_women.xlsx
+++ b/setuper/data/registration_vaccination_pregnant_women.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LaurePontis\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432A1997-6EE0-4294-B8D3-3B3B08FA4AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899D83AB-CBBE-420D-93EA-68DA181AE4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
   <si>
     <t>type</t>
   </si>
@@ -343,160 +343,13 @@
     <t>physiology</t>
   </si>
   <si>
-    <t>previous_muac</t>
-  </si>
-  <si>
-    <t>MUAC</t>
-  </si>
-  <si>
     <t>""</t>
   </si>
   <si>
-    <t>anthropometric_visit_done</t>
-  </si>
-  <si>
-    <t>Anthropometric visit is done</t>
-  </si>
-  <si>
-    <t>medical_visit_done</t>
-  </si>
-  <si>
-    <t>Medical visit is done</t>
-  </si>
-  <si>
-    <t>followup_visits</t>
-  </si>
-  <si>
-    <t>Follow up visits</t>
-  </si>
-  <si>
-    <t>prevous_muac_color</t>
-  </si>
-  <si>
-    <t>Muac color</t>
-  </si>
-  <si>
-    <t>program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Program </t>
-  </si>
-  <si>
-    <t>next_visit__date__</t>
-  </si>
-  <si>
-    <t>Next Visit Date</t>
-  </si>
-  <si>
-    <t>previous_soap_given</t>
-  </si>
-  <si>
-    <t>Soap given in last visit</t>
-  </si>
-  <si>
     <t>"no"</t>
   </si>
   <si>
-    <t>previous_net_given</t>
-  </si>
-  <si>
-    <t>Mosquito net given in last visit</t>
-  </si>
-  <si>
-    <t>previous_number_of_green_visits</t>
-  </si>
-  <si>
-    <t>Previous number of green visits</t>
-  </si>
-  <si>
-    <t>previous_number_of_yellow_visits</t>
-  </si>
-  <si>
-    <t>Previous number of yellow visits</t>
-  </si>
-  <si>
-    <t>previous_total_number_of_visits</t>
-  </si>
-  <si>
-    <t>Total number of visits</t>
-  </si>
-  <si>
-    <t>is_exiting</t>
-  </si>
-  <si>
-    <t>Is exiting</t>
-  </si>
-  <si>
-    <t>discharged_date__date__</t>
-  </si>
-  <si>
-    <t>Discharged date</t>
-  </si>
-  <si>
-    <t>is_pregnant</t>
-  </si>
-  <si>
     <t>Pregnant</t>
-  </si>
-  <si>
-    <t>is_breastfeeding</t>
-  </si>
-  <si>
-    <t>Breastfeeding</t>
-  </si>
-  <si>
-    <t>child_age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age (Months) </t>
-  </si>
-  <si>
-    <t>actual_child_birthday__date__</t>
-  </si>
-  <si>
-    <t>Actual Birthdate</t>
-  </si>
-  <si>
-    <t>cured__bool__</t>
-  </si>
-  <si>
-    <t>Cured</t>
-  </si>
-  <si>
-    <t>defaulter</t>
-  </si>
-  <si>
-    <t>Defaulter</t>
-  </si>
-  <si>
-    <t>pregnancy_child_age</t>
-  </si>
-  <si>
-    <t>Pregnancy age</t>
-  </si>
-  <si>
-    <t>transfer_to_ou_id</t>
-  </si>
-  <si>
-    <t>Transfer ou id</t>
-  </si>
-  <si>
-    <t>transfer_to_ou_name</t>
-  </si>
-  <si>
-    <t>Transfer ou name</t>
-  </si>
-  <si>
-    <t>org_unit_id</t>
-  </si>
-  <si>
-    <t>OU id</t>
-  </si>
-  <si>
-    <t>org_unit_name</t>
-  </si>
-  <si>
-    <t>OU  name</t>
   </si>
   <si>
     <t>list_name</t>
@@ -1179,8 +1032,8 @@
   <dimension ref="A1:AG999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1505,9 +1358,7 @@
       <c r="C8" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="26" t="s">
-        <v>28</v>
-      </c>
+      <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
@@ -1548,9 +1399,7 @@
       <c r="C9" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="26" t="s">
-        <v>28</v>
-      </c>
+      <c r="D9" s="26"/>
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
@@ -1669,13 +1518,13 @@
     </row>
     <row r="12" spans="1:33" ht="14.4">
       <c r="A12" s="26" t="s">
-        <v>199</v>
+        <v>150</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>200</v>
+        <v>151</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>201</v>
+        <v>152</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
@@ -1833,9 +1682,7 @@
       <c r="C16" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
@@ -1876,9 +1723,7 @@
       <c r="C17" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15" t="s">
         <v>54</v>
@@ -1925,9 +1770,7 @@
       <c r="C18" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15" t="s">
         <v>60</v>
@@ -1974,9 +1817,7 @@
       <c r="C19" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
@@ -2019,9 +1860,7 @@
       <c r="C20" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
@@ -2454,7 +2293,7 @@
         <v>83</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>193</v>
+        <v>144</v>
       </c>
       <c r="D31" s="37"/>
       <c r="E31" s="37" t="s">
@@ -2497,11 +2336,9 @@
         <v>84</v>
       </c>
       <c r="C32" s="56" t="s">
-        <v>198</v>
-      </c>
-      <c r="D32" s="37" t="s">
-        <v>28</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D32" s="37"/>
       <c r="E32" s="37"/>
       <c r="F32" s="37"/>
       <c r="G32" s="37"/>
@@ -2540,7 +2377,7 @@
         <v>86</v>
       </c>
       <c r="C33" s="56" t="s">
-        <v>197</v>
+        <v>148</v>
       </c>
       <c r="D33" s="37"/>
       <c r="E33" s="37"/>
@@ -2754,15 +2591,9 @@
       <c r="O39" s="41"/>
     </row>
     <row r="40" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A40" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>90</v>
-      </c>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
@@ -2773,21 +2604,15 @@
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
       <c r="M40" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N40" s="12"/>
       <c r="O40" s="12"/>
     </row>
     <row r="41" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A41" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>93</v>
-      </c>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
@@ -2815,15 +2640,9 @@
       <c r="Z41" s="11"/>
     </row>
     <row r="42" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A42" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>95</v>
-      </c>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
@@ -2851,15 +2670,9 @@
       <c r="Z42" s="11"/>
     </row>
     <row r="43" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A43" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>97</v>
-      </c>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
@@ -2887,15 +2700,9 @@
       <c r="Z43" s="11"/>
     </row>
     <row r="44" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A44" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>99</v>
-      </c>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
@@ -2906,21 +2713,15 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N44" s="12"/>
       <c r="O44" s="12"/>
     </row>
     <row r="45" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A45" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>101</v>
-      </c>
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
@@ -2931,21 +2732,15 @@
       <c r="K45" s="11"/>
       <c r="L45" s="11"/>
       <c r="M45" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N45" s="12"/>
       <c r="O45" s="12"/>
     </row>
     <row r="46" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A46" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" s="43" t="s">
-        <v>102</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>103</v>
-      </c>
+      <c r="A46" s="11"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
@@ -2956,21 +2751,15 @@
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N46" s="12"/>
       <c r="O46" s="12"/>
     </row>
     <row r="47" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A47" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>105</v>
-      </c>
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
@@ -2981,21 +2770,15 @@
       <c r="K47" s="11"/>
       <c r="L47" s="11"/>
       <c r="M47" s="11" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="N47" s="12"/>
       <c r="O47" s="12"/>
     </row>
     <row r="48" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A48" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>108</v>
-      </c>
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
@@ -3006,21 +2789,15 @@
       <c r="K48" s="11"/>
       <c r="L48" s="11"/>
       <c r="M48" s="11" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="N48" s="12"/>
       <c r="O48" s="12"/>
     </row>
     <row r="49" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A49" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>110</v>
-      </c>
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
@@ -3037,15 +2814,9 @@
       <c r="O49" s="12"/>
     </row>
     <row r="50" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A50" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
@@ -3062,15 +2833,9 @@
       <c r="O50" s="12"/>
     </row>
     <row r="51" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A51" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>114</v>
-      </c>
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
@@ -3087,15 +2852,9 @@
       <c r="O51" s="12"/>
     </row>
     <row r="52" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A52" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
@@ -3112,15 +2871,9 @@
       <c r="O52" s="12"/>
     </row>
     <row r="53" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A53" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>118</v>
-      </c>
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
@@ -3131,21 +2884,15 @@
       <c r="K53" s="11"/>
       <c r="L53" s="11"/>
       <c r="M53" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N53" s="12"/>
       <c r="O53" s="12"/>
     </row>
     <row r="54" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A54" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>120</v>
-      </c>
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
@@ -3156,21 +2903,15 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
       <c r="M54" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N54" s="12"/>
       <c r="O54" s="12"/>
     </row>
     <row r="55" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A55" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>122</v>
-      </c>
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
@@ -3181,21 +2922,15 @@
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
       <c r="M55" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N55" s="12"/>
       <c r="O55" s="12"/>
     </row>
     <row r="56" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A56" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B56" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>124</v>
-      </c>
+      <c r="A56" s="44"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="22"/>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
@@ -3212,15 +2947,9 @@
       <c r="O56" s="12"/>
     </row>
     <row r="57" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A57" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>126</v>
-      </c>
+      <c r="A57" s="44"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="22"/>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
@@ -3231,21 +2960,15 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
       <c r="M57" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N57" s="12"/>
       <c r="O57" s="12"/>
     </row>
     <row r="58" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A58" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>128</v>
-      </c>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
@@ -3280,15 +3003,9 @@
       <c r="AG58" s="11"/>
     </row>
     <row r="59" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A59" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="B59" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="C59" s="41" t="s">
-        <v>130</v>
-      </c>
+      <c r="A59" s="41"/>
+      <c r="B59" s="41"/>
+      <c r="C59" s="41"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
@@ -3323,15 +3040,9 @@
       <c r="AG59" s="11"/>
     </row>
     <row r="60" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A60" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B60" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>132</v>
-      </c>
+      <c r="A60" s="12"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="12"/>
       <c r="D60" s="12"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
@@ -3348,15 +3059,9 @@
       <c r="O60" s="12"/>
     </row>
     <row r="61" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A61" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B61" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="C61" s="41" t="s">
-        <v>134</v>
-      </c>
+      <c r="A61" s="8"/>
+      <c r="B61" s="41"/>
+      <c r="C61" s="41"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
       <c r="F61" s="11"/>
@@ -3391,15 +3096,9 @@
       <c r="AG61" s="11"/>
     </row>
     <row r="62" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A62" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B62" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="C62" s="41" t="s">
-        <v>136</v>
-      </c>
+      <c r="A62" s="8"/>
+      <c r="B62" s="41"/>
+      <c r="C62" s="41"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
@@ -3410,7 +3109,7 @@
       <c r="K62" s="11"/>
       <c r="L62" s="11"/>
       <c r="M62" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N62" s="11"/>
       <c r="O62" s="11"/>
@@ -3434,15 +3133,9 @@
       <c r="AG62" s="11"/>
     </row>
     <row r="63" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A63" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>138</v>
-      </c>
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
@@ -3477,15 +3170,9 @@
       <c r="AG63" s="11"/>
     </row>
     <row r="64" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A64" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>140</v>
-      </c>
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
@@ -3496,7 +3183,7 @@
       <c r="K64" s="11"/>
       <c r="L64" s="11"/>
       <c r="M64" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N64" s="11"/>
       <c r="O64" s="11"/>
@@ -7038,7 +6725,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
       <c r="B1" s="49" t="s">
         <v>1</v>
@@ -7050,7 +6737,7 @@
         <v>82</v>
       </c>
       <c r="E1" s="48" t="s">
-        <v>142</v>
+        <v>93</v>
       </c>
       <c r="F1" s="48"/>
       <c r="G1" s="48"/>
@@ -7075,13 +6762,13 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>144</v>
+        <v>95</v>
       </c>
       <c r="D2" s="48"/>
       <c r="E2" s="48"/>
@@ -7108,13 +6795,13 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="D3" s="48"/>
       <c r="E3" s="48"/>
@@ -7141,13 +6828,13 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="48"/>
@@ -7174,13 +6861,13 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="D5" s="48"/>
       <c r="E5" s="48"/>
@@ -7207,13 +6894,13 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>153</v>
+        <v>104</v>
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="48"/>
@@ -7240,13 +6927,13 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="12" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="D7" s="48"/>
       <c r="E7" s="48"/>
@@ -7276,10 +6963,10 @@
         <v>40</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
@@ -7287,7 +6974,7 @@
         <v>40</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>158</v>
+        <v>109</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>42</v>
@@ -7298,10 +6985,10 @@
         <v>88</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>159</v>
+        <v>110</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
@@ -7309,65 +6996,65 @@
         <v>88</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>161</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="12" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>163</v>
+        <v>114</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>164</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>165</v>
+        <v>116</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>166</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>167</v>
+        <v>118</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>168</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="12" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>169</v>
+        <v>120</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>170</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
@@ -7395,13 +7082,13 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>175</v>
+        <v>126</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
@@ -7429,35 +7116,35 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="50" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
       <c r="A19" s="50" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>179</v>
+        <v>130</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>180</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>182</v>
+        <v>133</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>194</v>
+        <v>145</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
@@ -7485,13 +7172,13 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="C21" s="55" t="s">
-        <v>195</v>
+        <v>146</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
@@ -7519,13 +7206,13 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="C22" s="55" t="s">
-        <v>196</v>
+        <v>147</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
@@ -7553,13 +7240,13 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>186</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1"/>
@@ -8558,17 +8245,17 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1">
       <c r="A1" s="39" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="D1" s="48"/>
       <c r="E1" s="48" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
       <c r="F1" s="48"/>
       <c r="G1" s="48"/>
@@ -8594,10 +8281,10 @@
         <v>28</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>191</v>
+        <v>142</v>
       </c>
       <c r="C2" s="53" t="s">
-        <v>192</v>
+        <v>143</v>
       </c>
       <c r="D2" s="48"/>
       <c r="E2" s="48"/>

</xml_diff>